<commit_message>
Changes in add HSIM menu
</commit_message>
<xml_diff>
--- a/testdata/SampleData.xlsx
+++ b/testdata/SampleData.xlsx
@@ -1,22 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28712"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vijay\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2655CF0E43E1348E/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9BFA4B-4411-4C6C-8831-2C09BDA52A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CF7EE46-32B1-4B35-A12E-5E46EF541A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2568" yWindow="1128" windowWidth="17280" windowHeight="10248" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="eDLFgBZR50WvvflsDPz1IH8KzUUUmAqDas49qeqv+rY="/>
     </ext>
@@ -36,20 +50,20 @@
     <t>res</t>
   </si>
   <si>
+    <t>BBSSL92</t>
+  </si>
+  <si>
+    <t>bbssl@123</t>
+  </si>
+  <si>
     <t>valid</t>
-  </si>
-  <si>
-    <t>BBSSL4</t>
-  </si>
-  <si>
-    <t>bbssl@123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -350,20 +364,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
-    <col min="2" max="2" width="55.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="55.7109375" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -374,18 +388,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{98961917-20C4-4C9C-B860-BCBFE47149F2}"/>

</xml_diff>